<commit_message>
Updated sessions in .xlsx
</commit_message>
<xml_diff>
--- a/NHP_TDCS_Behavior_Compiled.xlsx
+++ b/NHP_TDCS_Behavior_Compiled.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="4220" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="8080" yWindow="4040" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ACC" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,50 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Trials</t>
+  </si>
+  <si>
+    <t>Stim</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>Sham</t>
+  </si>
+  <si>
+    <t>Anodal</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>2 files</t>
+  </si>
+  <si>
+    <t>5min_pre</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58,8 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,14 +383,544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42838</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>836</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42838</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1725</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>2892</v>
+      </c>
+      <c r="G6">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42844</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>815</v>
+      </c>
+      <c r="G7">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42844</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42844</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>949</v>
+      </c>
+      <c r="G9">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42846</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>885</v>
+      </c>
+      <c r="G10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42846</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>993</v>
+      </c>
+      <c r="G11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42846</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42849</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>2665</v>
+      </c>
+      <c r="G13">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42849</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42849</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>892</v>
+      </c>
+      <c r="G15">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42849</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>801</v>
+      </c>
+      <c r="G16">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42851</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>1141</v>
+      </c>
+      <c r="G17">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42851</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42851</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>885</v>
+      </c>
+      <c r="G19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42851</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>859</v>
+      </c>
+      <c r="G20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1">
+        <v>42851</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>924</v>
+      </c>
+      <c r="G21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42851</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>795</v>
+      </c>
+      <c r="G22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42858</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>3553</v>
+      </c>
+      <c r="G23">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1">
+        <v>42858</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>1134</v>
+      </c>
+      <c r="G24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42858</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>858</v>
+      </c>
+      <c r="G25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1">
+        <v>42858</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>1034</v>
+      </c>
+      <c r="G26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>42865</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>2254</v>
+      </c>
+      <c r="G27">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42865</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>974</v>
+      </c>
+      <c r="G28">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <f>SUM(G4:G28)</f>
+        <v>12215</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Began commenting and constructing array
</commit_message>
<xml_diff>
--- a/NHP_TDCS_Behavior_Compiled.xlsx
+++ b/NHP_TDCS_Behavior_Compiled.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="4040" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="14180" yWindow="5540" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ACC" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t>Session</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>Gamma</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Abort (2651)</t>
+  </si>
+  <si>
+    <t>CorrectSaccade (2600)</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>incorrectSaccade (887)</t>
   </si>
 </sst>
 </file>
@@ -385,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -927,12 +942,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>